<commit_message>
removing some print statements
</commit_message>
<xml_diff>
--- a/SFR_Flux_Data.xlsx
+++ b/SFR_Flux_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\PycharmProjects\FNS_GA_v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1647DF-673A-4034-8F23-BF893C468D9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B992A0-1490-4354-BB42-60F4C920E728}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9740AB35-C658-4006-9BEA-5BE041493538}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9740AB35-C658-4006-9BEA-5BE041493538}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw_Data" sheetId="1" r:id="rId1"/>
@@ -4699,8 +4699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E06335DE-BD5C-4B2F-A9F8-41F8DFA26464}">
   <dimension ref="A1:G764"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="I247" sqref="I1:J1048576"/>
+    <sheetView topLeftCell="A233" workbookViewId="0">
+      <selection activeCell="H240" sqref="H240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20707,8 +20707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206DE899-CD5B-4A58-AEB7-70F3AF3A1774}">
   <dimension ref="A1:O760"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37935,8 +37935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A121C5BD-7170-4C15-95E3-A02876A81B38}">
   <dimension ref="A1:C253"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>